<commit_message>
Add course proj report
</commit_message>
<xml_diff>
--- a/Course project/research/clean_joined.xlsx
+++ b/Course project/research/clean_joined.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmitr\Desktop\6 сем\матстат\PolyMatStat\Course project\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335A45D2-D1AE-45EB-AAD5-75E40AE1D8A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67FC7462-5919-49DE-BA79-D51D9393792C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A1621B0F-C5A6-4DA6-93E0-208A22E1CC32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3386B8B-D48E-4F46-832B-53E9AF2376F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,236 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+  <si>
+    <t>probe</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>C2H6</t>
+  </si>
+  <si>
+    <t>C2H4</t>
+  </si>
+  <si>
+    <t>C3H8</t>
+  </si>
+  <si>
+    <t>C3H6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> i-C4H10</t>
+  </si>
+  <si>
+    <t>n-C4H10</t>
+  </si>
+  <si>
+    <t>C4H8</t>
+  </si>
+  <si>
+    <t>i-C4H8</t>
+  </si>
+  <si>
+    <t>i-C5H12</t>
+  </si>
+  <si>
+    <t>n-C5H12</t>
+  </si>
+  <si>
+    <t>03В</t>
+  </si>
+  <si>
+    <t>04В</t>
+  </si>
+  <si>
+    <t>05В</t>
+  </si>
+  <si>
+    <t>06В</t>
+  </si>
+  <si>
+    <t>08В</t>
+  </si>
+  <si>
+    <t>09В</t>
+  </si>
+  <si>
+    <t>10В</t>
+  </si>
+  <si>
+    <t>11В</t>
+  </si>
+  <si>
+    <t>13В</t>
+  </si>
+  <si>
+    <t>14В</t>
+  </si>
+  <si>
+    <t>15В</t>
+  </si>
+  <si>
+    <t>17В</t>
+  </si>
+  <si>
+    <t>18-03В_0-20</t>
+  </si>
+  <si>
+    <t>19В</t>
+  </si>
+  <si>
+    <t>20В</t>
+  </si>
+  <si>
+    <t>21В</t>
+  </si>
+  <si>
+    <t>22В</t>
+  </si>
+  <si>
+    <t>23В</t>
+  </si>
+  <si>
+    <t>24В</t>
+  </si>
+  <si>
+    <t>25В</t>
+  </si>
+  <si>
+    <t>26В</t>
+  </si>
+  <si>
+    <t>27В</t>
+  </si>
+  <si>
+    <t>28В</t>
+  </si>
+  <si>
+    <t>29В</t>
+  </si>
+  <si>
+    <t>30В</t>
+  </si>
+  <si>
+    <t>31В</t>
+  </si>
+  <si>
+    <t>32В</t>
+  </si>
+  <si>
+    <t>33В</t>
+  </si>
+  <si>
+    <t>34В</t>
+  </si>
+  <si>
+    <t>35В</t>
+  </si>
+  <si>
+    <t>36В</t>
+  </si>
+  <si>
+    <t>37В</t>
+  </si>
+  <si>
+    <t>39В</t>
+  </si>
+  <si>
+    <t>40В</t>
+  </si>
+  <si>
+    <t>41В</t>
+  </si>
+  <si>
+    <t>42В</t>
+  </si>
+  <si>
+    <t>43В</t>
+  </si>
+  <si>
+    <t>44В</t>
+  </si>
+  <si>
+    <t>45В</t>
+  </si>
+  <si>
+    <t>46В</t>
+  </si>
+  <si>
+    <t>47В</t>
+  </si>
+  <si>
+    <t>48В</t>
+  </si>
+  <si>
+    <t>49В</t>
+  </si>
+  <si>
+    <t>51В</t>
+  </si>
+  <si>
+    <t>52В</t>
+  </si>
+  <si>
+    <t>53В</t>
+  </si>
+  <si>
+    <t>55В</t>
+  </si>
+  <si>
+    <t>56В</t>
+  </si>
+  <si>
+    <t>17-01</t>
+  </si>
+  <si>
+    <t>17-02</t>
+  </si>
+  <si>
+    <t>17-03</t>
+  </si>
+  <si>
+    <t>17-04</t>
+  </si>
+  <si>
+    <t>17-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17-06 </t>
+  </si>
+  <si>
+    <t>17-07</t>
+  </si>
+  <si>
+    <t>17-08</t>
+  </si>
+  <si>
+    <t>17-09</t>
+  </si>
+  <si>
+    <t>17-10</t>
+  </si>
+  <si>
+    <t>17-11</t>
+  </si>
+  <si>
+    <t>17-12</t>
+  </si>
+  <si>
+    <t>17-18</t>
+  </si>
+  <si>
+    <t>17-19</t>
+  </si>
+  <si>
+    <t>17-26</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,2252 +612,2482 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4A2225-2B5D-46F4-914B-CFC34BC60EE8}">
-  <dimension ref="A1:K64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F7FDD7-83EE-4058-903A-C9941B886F9F}">
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
         <v>220.125958</v>
       </c>
-      <c r="B1">
+      <c r="C2">
         <v>17.286475999999997</v>
       </c>
-      <c r="C1">
+      <c r="D2">
         <v>6.2890289999999993</v>
       </c>
-      <c r="D1">
+      <c r="E2">
         <v>8.7938499999999991</v>
       </c>
-      <c r="E1">
+      <c r="F2">
         <v>3.7338409999999995</v>
       </c>
-      <c r="F1">
+      <c r="G2">
         <v>0.8221719999999999</v>
       </c>
-      <c r="G1">
+      <c r="H2">
         <v>3.0929249999999997</v>
       </c>
-      <c r="H1">
+      <c r="I2">
         <v>1.711174</v>
       </c>
-      <c r="I1">
+      <c r="J2">
         <v>1.8756409999999999</v>
       </c>
-      <c r="J1">
+      <c r="K2">
         <v>1.2405930000000001</v>
       </c>
-      <c r="K1">
+      <c r="L2">
         <v>1.177349</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
         <v>281.81124999999997</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>35.963875000000002</v>
       </c>
-      <c r="C2">
+      <c r="D3">
         <v>10.727625</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>15.475625000000001</v>
       </c>
-      <c r="E2">
+      <c r="F3">
         <v>7.3475000000000001</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>1.0342499999999999</v>
       </c>
-      <c r="G2">
+      <c r="H3">
         <v>5.0097499999999995</v>
       </c>
-      <c r="H2">
+      <c r="I3">
         <v>2.7061249999999997</v>
       </c>
-      <c r="I2">
+      <c r="J3">
         <v>2.0022499999999996</v>
       </c>
-      <c r="J2">
+      <c r="K3">
         <v>1.9558750000000003</v>
       </c>
-      <c r="K2">
+      <c r="L3">
         <v>2.0637500000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
         <v>139.42296899999999</v>
       </c>
-      <c r="B3">
+      <c r="C4">
         <v>8.1538310000000003</v>
       </c>
-      <c r="C3">
+      <c r="D4">
         <v>2.5530679999999997</v>
       </c>
-      <c r="D3">
+      <c r="E4">
         <v>3.5150570000000001</v>
       </c>
-      <c r="E3">
+      <c r="F4">
         <v>1.252461</v>
       </c>
-      <c r="F3">
+      <c r="G4">
         <v>0.29259999999999997</v>
       </c>
-      <c r="G3">
+      <c r="H4">
         <v>1.4090020000000001</v>
       </c>
-      <c r="H3">
+      <c r="I4">
         <v>0.51018799999999986</v>
       </c>
-      <c r="I3">
+      <c r="J4">
         <v>1.0733099999999998</v>
       </c>
-      <c r="J3">
+      <c r="K4">
         <v>0.91450799999999999</v>
       </c>
-      <c r="K3">
+      <c r="L4">
         <v>0.48385399999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
         <v>258.48186599999997</v>
       </c>
-      <c r="B4">
+      <c r="C5">
         <v>4.6878600000000006</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>1.2232320000000001</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>1.9274459999999995</v>
       </c>
-      <c r="E4">
+      <c r="F5">
         <v>0.29297400000000001</v>
       </c>
-      <c r="F4">
+      <c r="G5">
         <v>0.23791199999999993</v>
       </c>
-      <c r="G4">
+      <c r="H5">
         <v>0.90652200000000005</v>
       </c>
-      <c r="H4">
+      <c r="I5">
         <v>0.27655199999999996</v>
       </c>
-      <c r="I4">
+      <c r="J5">
         <v>1.0467299999999999</v>
       </c>
-      <c r="J4">
+      <c r="K5">
         <v>0.88637399999999988</v>
       </c>
-      <c r="K4">
+      <c r="L5">
         <v>0.20658600000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
         <v>155.650318</v>
       </c>
-      <c r="B5">
+      <c r="C6">
         <v>8.2585779999999982</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <v>2.511838</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <v>3.7458179999999999</v>
       </c>
-      <c r="E5">
+      <c r="F6">
         <v>1.3988419999999999</v>
       </c>
-      <c r="F5">
+      <c r="G6">
         <v>0.30842400000000003</v>
       </c>
-      <c r="G5">
+      <c r="H6">
         <v>1.3045539999999998</v>
       </c>
-      <c r="H5">
+      <c r="I6">
         <v>0.698214</v>
       </c>
-      <c r="I5">
+      <c r="J6">
         <v>1.163548</v>
       </c>
-      <c r="J5">
+      <c r="K6">
         <v>1.0168619999999999</v>
       </c>
-      <c r="K5">
+      <c r="L6">
         <v>0.47683599999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
         <v>191.77367999999998</v>
       </c>
-      <c r="B6">
+      <c r="C7">
         <v>18.19258</v>
       </c>
-      <c r="C6">
+      <c r="D7">
         <v>5.1197999999999997</v>
       </c>
-      <c r="D6">
+      <c r="E7">
         <v>8.328599999999998</v>
       </c>
-      <c r="E6">
+      <c r="F7">
         <v>3.6066799999999999</v>
       </c>
-      <c r="F6">
+      <c r="G7">
         <v>0.62831999999999999</v>
       </c>
-      <c r="G6">
+      <c r="H7">
         <v>2.85012</v>
       </c>
-      <c r="H6">
+      <c r="I7">
         <v>1.26868</v>
       </c>
-      <c r="I6">
+      <c r="J7">
         <v>1.33266</v>
       </c>
-      <c r="J6">
+      <c r="K7">
         <v>1.2296199999999999</v>
       </c>
-      <c r="K6">
+      <c r="L7">
         <v>1.2882799999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
         <v>113.23042500000001</v>
       </c>
-      <c r="B7">
+      <c r="C8">
         <v>5.8505700000000003</v>
       </c>
-      <c r="C7">
+      <c r="D8">
         <v>1.6617149999999996</v>
       </c>
-      <c r="D7">
+      <c r="E8">
         <v>2.9460749999999996</v>
       </c>
-      <c r="E7">
+      <c r="F8">
         <v>1.3079549999999998</v>
       </c>
-      <c r="F7">
+      <c r="G8">
         <v>0.25294500000000003</v>
       </c>
-      <c r="G7">
+      <c r="H8">
         <v>0.98372999999999999</v>
       </c>
-      <c r="H7">
+      <c r="I8">
         <v>1.44408</v>
       </c>
-      <c r="I7">
+      <c r="J8">
         <v>0</v>
       </c>
-      <c r="J7">
+      <c r="K8">
         <v>2.1223949999999996</v>
       </c>
-      <c r="K7">
+      <c r="L8">
         <v>0.59647500000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
         <v>121.12584</v>
       </c>
-      <c r="B8">
+      <c r="C9">
         <v>6.4666799999999993</v>
       </c>
-      <c r="C8">
+      <c r="D9">
         <v>1.696035</v>
       </c>
-      <c r="D8">
+      <c r="E9">
         <v>3.2551200000000002</v>
       </c>
-      <c r="E8">
+      <c r="F9">
         <v>1.3000349999999998</v>
       </c>
-      <c r="F8">
+      <c r="G9">
         <v>0.38692499999999996</v>
       </c>
-      <c r="G8">
+      <c r="H9">
         <v>1.11639</v>
       </c>
-      <c r="H8">
+      <c r="I9">
         <v>1.0952699999999997</v>
       </c>
-      <c r="I8">
+      <c r="J9">
         <v>0</v>
       </c>
-      <c r="J8">
+      <c r="K9">
         <v>1.7602199999999999</v>
       </c>
-      <c r="K8">
+      <c r="L9">
         <v>0.30392999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
         <v>166.49564999999996</v>
       </c>
-      <c r="B9">
+      <c r="C10">
         <v>6.4435499999999992</v>
       </c>
-      <c r="C9">
+      <c r="D10">
         <v>1.7301</v>
       </c>
-      <c r="D9">
+      <c r="E10">
         <v>2.9334000000000002</v>
       </c>
-      <c r="E9">
+      <c r="F10">
         <v>1.2928499999999998</v>
       </c>
-      <c r="F9">
+      <c r="G10">
         <v>0.23174999999999998</v>
       </c>
-      <c r="G9">
+      <c r="H10">
         <v>1.0700999999999998</v>
       </c>
-      <c r="H9">
+      <c r="I10">
         <v>0.58860000000000001</v>
       </c>
-      <c r="I9">
+      <c r="J10">
         <v>1.2492000000000001</v>
       </c>
-      <c r="J9">
+      <c r="K10">
         <v>1.3525499999999999</v>
       </c>
-      <c r="K9">
+      <c r="L10">
         <v>0.31439999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
         <v>192.92880399999996</v>
       </c>
-      <c r="B10">
+      <c r="C11">
         <v>4.4431079999999996</v>
       </c>
-      <c r="C10">
+      <c r="D11">
         <v>1.1684600000000001</v>
       </c>
-      <c r="D10">
+      <c r="E11">
         <v>2.0342599999999997</v>
       </c>
-      <c r="E10">
+      <c r="F11">
         <v>0.98597599999999996</v>
       </c>
-      <c r="F10">
+      <c r="G11">
         <v>0.27779599999999993</v>
       </c>
-      <c r="G10">
+      <c r="H11">
         <v>0.73970399999999992</v>
       </c>
-      <c r="H10">
+      <c r="I11">
         <v>0.28045999999999999</v>
       </c>
-      <c r="I10">
+      <c r="J11">
         <v>0.79120800000000002</v>
       </c>
-      <c r="J10">
+      <c r="K11">
         <v>0.62633600000000011</v>
       </c>
-      <c r="K10">
+      <c r="L11">
         <v>0.31657199999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
         <v>188.84448</v>
       </c>
-      <c r="B11">
+      <c r="C12">
         <v>4.0164299999999997</v>
       </c>
-      <c r="C11">
+      <c r="D12">
         <v>1.0533599999999999</v>
       </c>
-      <c r="D11">
+      <c r="E12">
         <v>1.9471649999999998</v>
       </c>
-      <c r="E11">
+      <c r="F12">
         <v>0.85420499999999999</v>
       </c>
-      <c r="F11">
+      <c r="G12">
         <v>0.22027500000000003</v>
       </c>
-      <c r="G11">
+      <c r="H12">
         <v>0.70108499999999996</v>
       </c>
-      <c r="H11">
+      <c r="I12">
         <v>0.2409</v>
       </c>
-      <c r="I11">
+      <c r="J12">
         <v>1.2637350000000001</v>
       </c>
-      <c r="J11">
+      <c r="K12">
         <v>1.1660550000000001</v>
       </c>
-      <c r="K11">
+      <c r="L12">
         <v>0.46414499999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
         <v>757.03530000000001</v>
       </c>
-      <c r="B12">
+      <c r="C13">
         <v>39.091360000000002</v>
       </c>
-      <c r="C12">
+      <c r="D13">
         <v>10.27642</v>
       </c>
-      <c r="D12">
+      <c r="E13">
         <v>17.591560000000001</v>
       </c>
-      <c r="E12">
+      <c r="F13">
         <v>7.8404199999999999</v>
       </c>
-      <c r="F12">
+      <c r="G13">
         <v>1.12574</v>
       </c>
-      <c r="G12">
+      <c r="H13">
         <v>5.6359799999999991</v>
       </c>
-      <c r="H12">
+      <c r="I13">
         <v>2.5076800000000001</v>
       </c>
-      <c r="I12">
+      <c r="J13">
         <v>2.5564</v>
       </c>
-      <c r="J12">
+      <c r="K13">
         <v>2.8769999999999998</v>
       </c>
-      <c r="K12">
+      <c r="L13">
         <v>1.5006599999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
         <v>61.398820000000001</v>
       </c>
-      <c r="B13">
+      <c r="C14">
         <v>2.0629000000000004</v>
       </c>
-      <c r="C13">
+      <c r="D14">
         <v>0.87891999999999992</v>
       </c>
-      <c r="D13">
+      <c r="E14">
         <v>0.41608000000000001</v>
       </c>
-      <c r="E13">
+      <c r="F14">
         <v>0.10038</v>
       </c>
-      <c r="F13">
+      <c r="G14">
         <v>0.21196000000000001</v>
       </c>
-      <c r="G13">
+      <c r="H14">
         <v>0.20061999999999999</v>
       </c>
-      <c r="H13">
+      <c r="I14">
         <v>5.8380000000000001E-2</v>
       </c>
-      <c r="I13">
+      <c r="J14">
         <v>1.5142399999999998</v>
       </c>
-      <c r="J13">
+      <c r="K14">
         <v>1.2864599999999999</v>
       </c>
-      <c r="K13">
+      <c r="L14">
         <v>0.54109999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
         <v>179.047225</v>
       </c>
-      <c r="B14">
+      <c r="C15">
         <v>4.3777999999999988</v>
       </c>
-      <c r="C14">
+      <c r="D15">
         <v>1.1726750000000001</v>
       </c>
-      <c r="D14">
+      <c r="E15">
         <v>2.1468999999999996</v>
       </c>
-      <c r="E14">
+      <c r="F15">
         <v>0.95777499999999993</v>
       </c>
-      <c r="F14">
+      <c r="G15">
         <v>0.24342500000000003</v>
       </c>
-      <c r="G14">
+      <c r="H15">
         <v>0.958125</v>
       </c>
-      <c r="H14">
+      <c r="I15">
         <v>0.56612499999999988</v>
       </c>
-      <c r="I14">
+      <c r="J15">
         <v>1.8110749999999998</v>
       </c>
-      <c r="J14">
+      <c r="K15">
         <v>1.6917250000000001</v>
       </c>
-      <c r="K14">
+      <c r="L15">
         <v>0.67584999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
         <v>149.72929399999998</v>
       </c>
-      <c r="B15">
+      <c r="C16">
         <v>3.569137</v>
       </c>
-      <c r="C15">
+      <c r="D16">
         <v>0.43157399999999996</v>
       </c>
-      <c r="D15">
+      <c r="E16">
         <v>1.9536659999999999</v>
       </c>
-      <c r="E15">
+      <c r="F16">
         <v>0.42842800000000003</v>
       </c>
-      <c r="F15">
+      <c r="G16">
         <v>0.25096499999999999</v>
       </c>
-      <c r="G15">
+      <c r="H16">
         <v>1.109108</v>
       </c>
-      <c r="H15">
+      <c r="I16">
         <v>0.64922000000000002</v>
       </c>
-      <c r="I15">
+      <c r="J16">
         <v>1.1282699999999999</v>
       </c>
-      <c r="J15">
+      <c r="K16">
         <v>0.72243599999999997</v>
       </c>
-      <c r="K15">
+      <c r="L16">
         <v>0.23738000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
         <v>167.57944199999997</v>
       </c>
-      <c r="B16">
+      <c r="C17">
         <v>4.1838119999999996</v>
       </c>
-      <c r="C16">
+      <c r="D17">
         <v>1.1730419999999999</v>
       </c>
-      <c r="D16">
+      <c r="E17">
         <v>1.909818</v>
       </c>
-      <c r="E16">
+      <c r="F17">
         <v>0.81680399999999997</v>
       </c>
-      <c r="F16">
+      <c r="G17">
         <v>0.19618199999999997</v>
       </c>
-      <c r="G16">
+      <c r="H17">
         <v>0.64718999999999993</v>
       </c>
-      <c r="H16">
+      <c r="I17">
         <v>0.42946199999999995</v>
       </c>
-      <c r="I16">
+      <c r="J17">
         <v>1.1673719999999999</v>
       </c>
-      <c r="J16">
+      <c r="K17">
         <v>1.4579999999999997</v>
       </c>
-      <c r="K16">
+      <c r="L17">
         <v>0.39479400000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
         <v>65.647805000000005</v>
       </c>
-      <c r="B17">
+      <c r="C18">
         <v>5.18703</v>
       </c>
-      <c r="C17">
+      <c r="D18">
         <v>1.3382900000000002</v>
       </c>
-      <c r="D17">
+      <c r="E18">
         <v>2.4366349999999994</v>
       </c>
-      <c r="E17">
+      <c r="F18">
         <v>1.0119499999999999</v>
       </c>
-      <c r="F17">
+      <c r="G18">
         <v>0.23383999999999999</v>
       </c>
-      <c r="G17">
+      <c r="H18">
         <v>1.0047349999999999</v>
       </c>
-      <c r="H17">
+      <c r="I18">
         <v>0.76293999999999995</v>
       </c>
-      <c r="I17">
+      <c r="J18">
         <v>1.7822899999999997</v>
       </c>
-      <c r="J17">
+      <c r="K18">
         <v>1.1745650000000003</v>
       </c>
-      <c r="K17">
+      <c r="L18">
         <v>0.38183999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19">
         <v>67.567040000000006</v>
       </c>
-      <c r="B18">
+      <c r="C19">
         <v>4.8761599999999996</v>
       </c>
-      <c r="C18">
+      <c r="D19">
         <v>1.35632</v>
       </c>
-      <c r="D18">
+      <c r="E19">
         <v>2.18784</v>
       </c>
-      <c r="E18">
+      <c r="F19">
         <v>0.82320000000000004</v>
       </c>
-      <c r="F18">
+      <c r="G19">
         <v>0.19904000000000002</v>
       </c>
-      <c r="G18">
+      <c r="H19">
         <v>0.76624000000000003</v>
       </c>
-      <c r="H18">
+      <c r="I19">
         <v>0.41647999999999991</v>
       </c>
-      <c r="I18">
+      <c r="J19">
         <v>1.47936</v>
       </c>
-      <c r="J18">
+      <c r="K19">
         <v>1.5638399999999999</v>
       </c>
-      <c r="K18">
+      <c r="L19">
         <v>0.25775999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
         <v>66.959599999999995</v>
       </c>
-      <c r="B19">
+      <c r="C20">
         <v>4.7042000000000002</v>
       </c>
-      <c r="C19">
+      <c r="D20">
         <v>1.2136</v>
       </c>
-      <c r="D19">
+      <c r="E20">
         <v>2.2057999999999995</v>
       </c>
-      <c r="E19">
+      <c r="F20">
         <v>0.92679999999999996</v>
       </c>
-      <c r="F19">
+      <c r="G20">
         <v>0.38900000000000001</v>
       </c>
-      <c r="G19">
+      <c r="H20">
         <v>1.1579999999999999</v>
       </c>
-      <c r="H19">
+      <c r="I20">
         <v>0.61280000000000012</v>
       </c>
-      <c r="I19">
+      <c r="J20">
         <v>2.9143999999999997</v>
       </c>
-      <c r="J19">
+      <c r="K20">
         <v>2.5961999999999996</v>
       </c>
-      <c r="K19">
+      <c r="L20">
         <v>0.56120000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
         <v>285.09812999999991</v>
       </c>
-      <c r="B20">
+      <c r="C21">
         <v>20.102418</v>
       </c>
-      <c r="C20">
+      <c r="D21">
         <v>3.534354</v>
       </c>
-      <c r="D20">
+      <c r="E21">
         <v>8.5868100000000016</v>
       </c>
-      <c r="E20">
+      <c r="F21">
         <v>2.7355320000000001</v>
       </c>
-      <c r="F20">
+      <c r="G21">
         <v>0.25498800000000005</v>
       </c>
-      <c r="G20">
+      <c r="H21">
         <v>2.5082459999999998</v>
       </c>
-      <c r="H20">
+      <c r="I21">
         <v>1.066932</v>
       </c>
-      <c r="I20">
+      <c r="J21">
         <v>1.6452719999999998</v>
       </c>
-      <c r="J20">
+      <c r="K21">
         <v>2.3700600000000001</v>
       </c>
-      <c r="K20">
+      <c r="L21">
         <v>1.144692</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
         <v>114.07522</v>
       </c>
-      <c r="B21">
+      <c r="C22">
         <v>5.3122999999999996</v>
       </c>
-      <c r="C21">
+      <c r="D22">
         <v>1.2944399999999998</v>
       </c>
-      <c r="D21">
+      <c r="E22">
         <v>2.3722999999999996</v>
       </c>
-      <c r="E21">
+      <c r="F22">
         <v>0.97650000000000015</v>
       </c>
-      <c r="F21">
+      <c r="G22">
         <v>0.22022</v>
       </c>
-      <c r="G21">
+      <c r="H22">
         <v>0.99721999999999988</v>
       </c>
-      <c r="H21">
+      <c r="I22">
         <v>0.25675999999999999</v>
       </c>
-      <c r="I21">
+      <c r="J22">
         <v>1.2020400000000002</v>
       </c>
-      <c r="J21">
+      <c r="K22">
         <v>1.44886</v>
       </c>
-      <c r="K21">
+      <c r="L22">
         <v>0.26501999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
         <v>296.85552000000001</v>
       </c>
-      <c r="B22">
+      <c r="C23">
         <v>4.3791999999999991</v>
       </c>
-      <c r="C22">
+      <c r="D23">
         <v>1.05504</v>
       </c>
-      <c r="D22">
+      <c r="E23">
         <v>1.9919999999999998</v>
       </c>
-      <c r="E22">
+      <c r="F23">
         <v>0.65359999999999996</v>
       </c>
-      <c r="F22">
+      <c r="G23">
         <v>0.20047999999999999</v>
       </c>
-      <c r="G22">
+      <c r="H23">
         <v>0.69567999999999997</v>
       </c>
-      <c r="H22">
+      <c r="I23">
         <v>0.39584000000000003</v>
       </c>
-      <c r="I22">
+      <c r="J23">
         <v>0.95504</v>
       </c>
-      <c r="J22">
+      <c r="K23">
         <v>0.92608000000000001</v>
       </c>
-      <c r="K22">
+      <c r="L23">
         <v>0.42415999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
         <v>397.53735000000006</v>
       </c>
-      <c r="B23">
+      <c r="C24">
         <v>1.4853000000000001</v>
       </c>
-      <c r="C23">
+      <c r="D24">
         <v>0.21479999999999996</v>
       </c>
-      <c r="D23">
+      <c r="E24">
         <v>1.5976499999999998</v>
       </c>
-      <c r="E23">
+      <c r="F24">
         <v>0.63285000000000002</v>
       </c>
-      <c r="F23">
+      <c r="G24">
         <v>0.20069999999999999</v>
       </c>
-      <c r="G23">
+      <c r="H24">
         <v>0.61964999999999992</v>
       </c>
-      <c r="H23">
+      <c r="I24">
         <v>0.17415</v>
       </c>
-      <c r="I23">
+      <c r="J24">
         <v>1.2940499999999999</v>
       </c>
-      <c r="J23">
+      <c r="K24">
         <v>1.9761</v>
       </c>
-      <c r="K23">
+      <c r="L24">
         <v>0.29309999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
         <v>650.70489399999985</v>
       </c>
-      <c r="B24">
+      <c r="C25">
         <v>4.9325240000000008</v>
       </c>
-      <c r="C24">
+      <c r="D25">
         <v>0.97757399999999983</v>
       </c>
-      <c r="D24">
+      <c r="E25">
         <v>2.1415660000000001</v>
       </c>
-      <c r="E24">
+      <c r="F25">
         <v>0.8902580000000001</v>
       </c>
-      <c r="F24">
+      <c r="G25">
         <v>0.53817199999999998</v>
       </c>
-      <c r="G24">
+      <c r="H25">
         <v>1.1608380000000003</v>
       </c>
-      <c r="H24">
+      <c r="I25">
         <v>0.50098799999999988</v>
       </c>
-      <c r="I24">
+      <c r="J25">
         <v>0.95350399999999991</v>
       </c>
-      <c r="J24">
+      <c r="K25">
         <v>0.93474600000000008</v>
       </c>
-      <c r="K24">
+      <c r="L25">
         <v>0.39258999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26">
         <v>1037.2086449999999</v>
       </c>
-      <c r="B25">
+      <c r="C26">
         <v>6.0404850000000003</v>
       </c>
-      <c r="C25">
+      <c r="D26">
         <v>1.4510099999999999</v>
       </c>
-      <c r="D25">
+      <c r="E26">
         <v>2.5142699999999998</v>
       </c>
-      <c r="E25">
+      <c r="F26">
         <v>0.93620999999999999</v>
       </c>
-      <c r="F25">
+      <c r="G26">
         <v>0.24766499999999997</v>
       </c>
-      <c r="G25">
+      <c r="H26">
         <v>1.0370250000000001</v>
       </c>
-      <c r="H25">
+      <c r="I26">
         <v>0.20360999999999999</v>
       </c>
-      <c r="I25">
+      <c r="J26">
         <v>1.3312200000000001</v>
       </c>
-      <c r="J25">
+      <c r="K26">
         <v>1.2305699999999997</v>
       </c>
-      <c r="K25">
+      <c r="L26">
         <v>0.68623500000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27">
         <v>604.78294500000004</v>
       </c>
-      <c r="B26">
+      <c r="C27">
         <v>4.8582850000000004</v>
       </c>
-      <c r="C26">
+      <c r="D27">
         <v>1.2892649999999999</v>
       </c>
-      <c r="D26">
+      <c r="E27">
         <v>2.3644850000000002</v>
       </c>
-      <c r="E26">
+      <c r="F27">
         <v>0.68135499999999993</v>
       </c>
-      <c r="F26">
+      <c r="G27">
         <v>0.31875500000000001</v>
       </c>
-      <c r="G26">
+      <c r="H27">
         <v>0.63991500000000001</v>
       </c>
-      <c r="H26">
+      <c r="I27">
         <v>0.18388999999999997</v>
       </c>
-      <c r="I26">
+      <c r="J27">
         <v>0.445295</v>
       </c>
-      <c r="J26">
+      <c r="K27">
         <v>1.2524499999999998</v>
       </c>
-      <c r="K26">
+      <c r="L27">
         <v>0.31801499999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28">
         <v>215.038051</v>
       </c>
-      <c r="B27">
+      <c r="C28">
         <v>3.5702239999999996</v>
       </c>
-      <c r="C27">
+      <c r="D28">
         <v>0.71107299999999996</v>
       </c>
-      <c r="D27">
+      <c r="E28">
         <v>2.2994619999999997</v>
       </c>
-      <c r="E27">
+      <c r="F28">
         <v>0.83400900000000011</v>
       </c>
-      <c r="F27">
+      <c r="G28">
         <v>1.370584</v>
       </c>
-      <c r="G27">
+      <c r="H28">
         <v>3.5736529999999997</v>
       </c>
-      <c r="H27">
+      <c r="I28">
         <v>0.15087600000000001</v>
       </c>
-      <c r="I27">
+      <c r="J28">
         <v>0.42887900000000001</v>
       </c>
-      <c r="J27">
+      <c r="K28">
         <v>1.4823440000000001</v>
       </c>
-      <c r="K27">
+      <c r="L28">
         <v>0.35839399999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
         <v>470.41441399999997</v>
       </c>
-      <c r="B28">
+      <c r="C29">
         <v>19.247366</v>
       </c>
-      <c r="C28">
+      <c r="D29">
         <v>4.0142009999999999</v>
       </c>
-      <c r="D28">
+      <c r="E29">
         <v>8.2535049999999988</v>
       </c>
-      <c r="E28">
+      <c r="F29">
         <v>3.1134629999999999</v>
       </c>
-      <c r="F28">
+      <c r="G29">
         <v>0.56039400000000006</v>
       </c>
-      <c r="G28">
+      <c r="H29">
         <v>2.2335889999999998</v>
       </c>
-      <c r="H28">
+      <c r="I29">
         <v>0.82152000000000003</v>
       </c>
-      <c r="I28">
+      <c r="J29">
         <v>0.68606699999999998</v>
       </c>
-      <c r="J28">
+      <c r="K29">
         <v>1.5630069999999998</v>
       </c>
-      <c r="K28">
+      <c r="L29">
         <v>0.59413499999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30">
         <v>407.50089000000008</v>
       </c>
-      <c r="B29">
+      <c r="C30">
         <v>4.3975080000000002</v>
       </c>
-      <c r="C29">
+      <c r="D30">
         <v>0.88913399999999998</v>
       </c>
-      <c r="D29">
+      <c r="E30">
         <v>1.7786820000000001</v>
       </c>
-      <c r="E29">
+      <c r="F30">
         <v>0.83269199999999999</v>
       </c>
-      <c r="F29">
+      <c r="G30">
         <v>0.22673399999999996</v>
       </c>
-      <c r="G29">
+      <c r="H30">
         <v>0.97483200000000003</v>
       </c>
-      <c r="H29">
+      <c r="I30">
         <v>0.24122399999999999</v>
       </c>
-      <c r="I29">
+      <c r="J30">
         <v>0.44780999999999993</v>
       </c>
-      <c r="J29">
+      <c r="K30">
         <v>0.7939139999999999</v>
       </c>
-      <c r="K29">
+      <c r="L30">
         <v>0.410136</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31">
         <v>145.64510399999998</v>
       </c>
-      <c r="B30">
+      <c r="C31">
         <v>4.3149759999999997</v>
       </c>
-      <c r="C30">
+      <c r="D31">
         <v>1.0054239999999999</v>
       </c>
-      <c r="D30">
+      <c r="E31">
         <v>1.8892119999999999</v>
       </c>
-      <c r="E30">
+      <c r="F31">
         <v>0.82832799999999995</v>
       </c>
-      <c r="F30">
+      <c r="G31">
         <v>0.30907200000000001</v>
       </c>
-      <c r="G30">
+      <c r="H31">
         <v>1.1667279999999998</v>
       </c>
-      <c r="H30">
+      <c r="I31">
         <v>0.41416399999999998</v>
       </c>
-      <c r="I30">
+      <c r="J31">
         <v>1.1840239999999995</v>
       </c>
-      <c r="J30">
+      <c r="K31">
         <v>1.3293479999999998</v>
       </c>
-      <c r="K30">
+      <c r="L31">
         <v>1.3400639999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32">
         <v>740.9320469999999</v>
       </c>
-      <c r="B31">
+      <c r="C32">
         <v>5.7817020000000001</v>
       </c>
-      <c r="C31">
+      <c r="D32">
         <v>1.2645299999999999</v>
       </c>
-      <c r="D31">
+      <c r="E32">
         <v>2.4145020000000001</v>
       </c>
-      <c r="E31">
+      <c r="F32">
         <v>1.013271</v>
       </c>
-      <c r="F31">
+      <c r="G32">
         <v>0.33122999999999997</v>
       </c>
-      <c r="G31">
+      <c r="H32">
         <v>1.089399</v>
       </c>
-      <c r="H31">
+      <c r="I32">
         <v>0.33598800000000001</v>
       </c>
-      <c r="I31">
+      <c r="J32">
         <v>1.216218</v>
       </c>
-      <c r="J31">
+      <c r="K32">
         <v>1.4316089999999999</v>
       </c>
-      <c r="K31">
+      <c r="L32">
         <v>0.57205799999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
         <v>713.14853399999993</v>
       </c>
-      <c r="B32">
+      <c r="C33">
         <v>3.8434379999999999</v>
       </c>
-      <c r="C32">
+      <c r="D33">
         <v>0.71539199999999992</v>
       </c>
-      <c r="D32">
+      <c r="E33">
         <v>1.5070979999999998</v>
       </c>
-      <c r="E32">
+      <c r="F33">
         <v>0.41620799999999997</v>
       </c>
-      <c r="F32">
+      <c r="G33">
         <v>0.19112999999999999</v>
       </c>
-      <c r="G32">
+      <c r="H33">
         <v>0.64032</v>
       </c>
-      <c r="H32">
+      <c r="I33">
         <v>0.28027800000000003</v>
       </c>
-      <c r="I32">
+      <c r="J33">
         <v>0.99346199999999985</v>
       </c>
-      <c r="J32">
+      <c r="K33">
         <v>0.92294399999999988</v>
       </c>
-      <c r="K32">
+      <c r="L33">
         <v>0.23266800000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34">
         <v>252.33957000000004</v>
       </c>
-      <c r="B33">
+      <c r="C34">
         <v>6.810719999999999</v>
       </c>
-      <c r="C33">
+      <c r="D34">
         <v>1.6293900000000003</v>
       </c>
-      <c r="D33">
+      <c r="E34">
         <v>2.8591499999999996</v>
       </c>
-      <c r="E33">
+      <c r="F34">
         <v>1.1493300000000002</v>
       </c>
-      <c r="F33">
+      <c r="G34">
         <v>0.31646999999999997</v>
       </c>
-      <c r="G33">
+      <c r="H34">
         <v>1.10754</v>
       </c>
-      <c r="H33">
+      <c r="I34">
         <v>0.60542999999999991</v>
       </c>
-      <c r="I33">
+      <c r="J34">
         <v>1.2495000000000001</v>
       </c>
-      <c r="J33">
+      <c r="K34">
         <v>1.63317</v>
       </c>
-      <c r="K33">
+      <c r="L34">
         <v>0.55524000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35">
         <v>451.14612399999999</v>
       </c>
-      <c r="B34">
+      <c r="C35">
         <v>4.2205399999999997</v>
       </c>
-      <c r="C34">
+      <c r="D35">
         <v>0.82984000000000002</v>
       </c>
-      <c r="D34">
+      <c r="E35">
         <v>1.6900200000000001</v>
       </c>
-      <c r="E34">
+      <c r="F35">
         <v>0.63139999999999996</v>
       </c>
-      <c r="F34">
+      <c r="G35">
         <v>0.35653599999999991</v>
       </c>
-      <c r="G34">
+      <c r="H35">
         <v>0.76505999999999996</v>
       </c>
-      <c r="H34">
+      <c r="I35">
         <v>0.69240799999999991</v>
       </c>
-      <c r="I34">
+      <c r="J35">
         <v>1.0784640000000001</v>
       </c>
-      <c r="J34">
+      <c r="K35">
         <v>1.0924039999999999</v>
       </c>
-      <c r="K34">
+      <c r="L35">
         <v>0.34439999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36">
         <v>2385.4197839999997</v>
       </c>
-      <c r="B35">
+      <c r="C36">
         <v>6.4801679999999999</v>
       </c>
-      <c r="C35">
+      <c r="D36">
         <v>1.397899</v>
       </c>
-      <c r="D35">
+      <c r="E36">
         <v>2.3484239999999996</v>
       </c>
-      <c r="E35">
+      <c r="F36">
         <v>0.69402799999999998</v>
       </c>
-      <c r="F35">
+      <c r="G36">
         <v>0.34913699999999998</v>
       </c>
-      <c r="G35">
+      <c r="H36">
         <v>0.96654399999999996</v>
       </c>
-      <c r="H35">
+      <c r="I36">
         <v>0.33427600000000002</v>
       </c>
-      <c r="I35">
+      <c r="J36">
         <v>1.27959</v>
       </c>
-      <c r="J35">
+      <c r="K36">
         <v>1.1705450000000002</v>
       </c>
-      <c r="K35">
+      <c r="L36">
         <v>0.36438399999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37">
         <v>166.073836</v>
       </c>
-      <c r="B36">
+      <c r="C37">
         <v>13.369463999999997</v>
       </c>
-      <c r="C36">
+      <c r="D37">
         <v>2.5632519999999999</v>
       </c>
-      <c r="D36">
+      <c r="E37">
         <v>5.6155599999999994</v>
       </c>
-      <c r="E36">
+      <c r="F37">
         <v>1.869804</v>
       </c>
-      <c r="F36">
+      <c r="G37">
         <v>0.35855599999999999</v>
       </c>
-      <c r="G36">
+      <c r="H37">
         <v>1.663788</v>
       </c>
-      <c r="H36">
+      <c r="I37">
         <v>0.593804</v>
       </c>
-      <c r="I36">
+      <c r="J37">
         <v>1.0178999999999998</v>
       </c>
-      <c r="J36">
+      <c r="K37">
         <v>1.2237999999999998</v>
       </c>
-      <c r="K36">
+      <c r="L37">
         <v>0.57895600000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38">
         <v>133.65121200000002</v>
       </c>
-      <c r="B37">
+      <c r="C38">
         <v>5.786459999999999</v>
       </c>
-      <c r="C37">
+      <c r="D38">
         <v>1.2319560000000001</v>
       </c>
-      <c r="D37">
+      <c r="E38">
         <v>2.2958160000000003</v>
       </c>
-      <c r="E37">
+      <c r="F38">
         <v>1.0591679999999999</v>
       </c>
-      <c r="F37">
+      <c r="G38">
         <v>0.39861600000000003</v>
       </c>
-      <c r="G37">
+      <c r="H38">
         <v>1.0920119999999998</v>
       </c>
-      <c r="H37">
+      <c r="I38">
         <v>0.48592800000000003</v>
       </c>
-      <c r="I37">
+      <c r="J38">
         <v>1.3578239999999999</v>
       </c>
-      <c r="J37">
+      <c r="K38">
         <v>1.5091920000000001</v>
       </c>
-      <c r="K37">
+      <c r="L38">
         <v>0.79498800000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39">
         <v>56.415374999999997</v>
       </c>
-      <c r="B38">
+      <c r="C39">
         <v>4.3529999999999998</v>
       </c>
-      <c r="C38">
+      <c r="D39">
         <v>0.82524999999999993</v>
       </c>
-      <c r="D38">
+      <c r="E39">
         <v>1.6464999999999999</v>
       </c>
-      <c r="E38">
+      <c r="F39">
         <v>0.43224999999999997</v>
       </c>
-      <c r="F38">
+      <c r="G39">
         <v>4.6375000000000006E-2</v>
       </c>
-      <c r="G38">
+      <c r="H39">
         <v>0.5472499999999999</v>
       </c>
-      <c r="H38">
+      <c r="I39">
         <v>0.139375</v>
       </c>
-      <c r="I38">
+      <c r="J39">
         <v>0.64787499999999998</v>
       </c>
-      <c r="J38">
+      <c r="K39">
         <v>1.0495000000000001</v>
       </c>
-      <c r="K38">
+      <c r="L39">
         <v>0.40787499999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40">
         <v>57.62530799999999</v>
       </c>
-      <c r="B39">
+      <c r="C40">
         <v>4.3388279999999995</v>
       </c>
-      <c r="C39">
+      <c r="D40">
         <v>0.74458799999999992</v>
       </c>
-      <c r="D39">
+      <c r="E40">
         <v>1.4660099999999998</v>
       </c>
-      <c r="E39">
+      <c r="F40">
         <v>0.31917599999999996</v>
       </c>
-      <c r="F39">
+      <c r="G40">
         <v>6.0956999999999997E-2</v>
       </c>
-      <c r="G39">
+      <c r="H40">
         <v>0.38621699999999992</v>
       </c>
-      <c r="H39">
+      <c r="I40">
         <v>9.2079000000000008E-2</v>
       </c>
-      <c r="I39">
+      <c r="J40">
         <v>0.65648700000000004</v>
       </c>
-      <c r="J39">
+      <c r="K40">
         <v>0.15748199999999998</v>
       </c>
-      <c r="K39">
+      <c r="L40">
         <v>0.161694</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41">
         <v>82.477667999999994</v>
       </c>
-      <c r="B40">
+      <c r="C41">
         <v>4.4886659999999994</v>
       </c>
-      <c r="C40">
+      <c r="D41">
         <v>1.0517780000000001</v>
       </c>
-      <c r="D40">
+      <c r="E41">
         <v>1.469104</v>
       </c>
-      <c r="E40">
+      <c r="F41">
         <v>0.48320999999999992</v>
       </c>
-      <c r="F40">
+      <c r="G41">
         <v>0.11283999999999998</v>
       </c>
-      <c r="G40">
+      <c r="H41">
         <v>0.64464399999999988</v>
       </c>
-      <c r="H40">
+      <c r="I41">
         <v>0.356902</v>
       </c>
-      <c r="I40">
+      <c r="J41">
         <v>0.90071800000000002</v>
       </c>
-      <c r="J40">
+      <c r="K41">
         <v>1.500772</v>
       </c>
-      <c r="K40">
+      <c r="L41">
         <v>0.25680199999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42">
         <v>88.516980000000004</v>
       </c>
-      <c r="B41">
+      <c r="C42">
         <v>7.01898</v>
       </c>
-      <c r="C41">
+      <c r="D42">
         <v>1.5058799999999999</v>
       </c>
-      <c r="D41">
+      <c r="E42">
         <v>2.588384</v>
       </c>
-      <c r="E41">
+      <c r="F42">
         <v>0.63807199999999997</v>
       </c>
-      <c r="F41">
+      <c r="G42">
         <v>0.12501999999999999</v>
       </c>
-      <c r="G41">
+      <c r="H42">
         <v>0.75275199999999998</v>
       </c>
-      <c r="H41">
+      <c r="I42">
         <v>0.24722000000000002</v>
       </c>
-      <c r="I41">
+      <c r="J42">
         <v>0.9997839999999999</v>
       </c>
-      <c r="J41">
+      <c r="K42">
         <v>1.774532</v>
       </c>
-      <c r="K41">
+      <c r="L42">
         <v>0.17784800000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43">
         <v>162.12401</v>
       </c>
-      <c r="B42">
+      <c r="C43">
         <v>5.5038999999999989</v>
       </c>
-      <c r="C42">
+      <c r="D43">
         <v>0.82443500000000003</v>
       </c>
-      <c r="D42">
+      <c r="E43">
         <v>2.1126649999999998</v>
       </c>
-      <c r="E42">
+      <c r="F43">
         <v>0.54682499999999989</v>
       </c>
-      <c r="F42">
+      <c r="G43">
         <v>0.11856499999999998</v>
       </c>
-      <c r="G42">
+      <c r="H43">
         <v>0.69034499999999999</v>
       </c>
-      <c r="H42">
+      <c r="I43">
         <v>0.19757</v>
       </c>
-      <c r="I42">
+      <c r="J43">
         <v>0.65434999999999988</v>
       </c>
-      <c r="J42">
+      <c r="K43">
         <v>1.2298099999999998</v>
       </c>
-      <c r="K42">
+      <c r="L43">
         <v>0.26035999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44">
         <v>221.748177</v>
       </c>
-      <c r="B43">
+      <c r="C44">
         <v>5.190275999999999</v>
       </c>
-      <c r="C43">
+      <c r="D44">
         <v>0.733236</v>
       </c>
-      <c r="D43">
+      <c r="E44">
         <v>1.7329829999999999</v>
       </c>
-      <c r="E43">
+      <c r="F44">
         <v>0.42806399999999994</v>
       </c>
-      <c r="F43">
+      <c r="G44">
         <v>0.27018599999999998</v>
       </c>
-      <c r="G43">
+      <c r="H44">
         <v>0.66782099999999989</v>
       </c>
-      <c r="H43">
+      <c r="I44">
         <v>0.36015000000000003</v>
       </c>
-      <c r="I43">
+      <c r="J44">
         <v>0.92815799999999993</v>
       </c>
-      <c r="J43">
+      <c r="K44">
         <v>1.516011</v>
       </c>
-      <c r="K43">
+      <c r="L44">
         <v>0.18992399999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45">
         <v>146.88464999999999</v>
       </c>
-      <c r="B44">
+      <c r="C45">
         <v>16.884599999999999</v>
       </c>
-      <c r="C44">
+      <c r="D45">
         <v>4.359375</v>
       </c>
-      <c r="D44">
+      <c r="E45">
         <v>5.8624499999999999</v>
       </c>
-      <c r="E44">
+      <c r="F45">
         <v>3.2179499999999996</v>
       </c>
-      <c r="F44">
+      <c r="G45">
         <v>0.23797499999999999</v>
       </c>
-      <c r="G44">
+      <c r="H45">
         <v>1.4528249999999998</v>
       </c>
-      <c r="H44">
+      <c r="I45">
         <v>0.8985749999999999</v>
       </c>
-      <c r="I44">
+      <c r="J45">
         <v>0.68354999999999988</v>
       </c>
-      <c r="J44">
+      <c r="K45">
         <v>1.3047</v>
       </c>
-      <c r="K44">
+      <c r="L45">
         <v>0.38452500000000006</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46">
         <v>72.391311999999999</v>
       </c>
-      <c r="B45">
+      <c r="C46">
         <v>6.5743999999999998</v>
       </c>
-      <c r="C45">
+      <c r="D46">
         <v>1.4092959999999997</v>
       </c>
-      <c r="D45">
+      <c r="E46">
         <v>2.4923359999999999</v>
       </c>
-      <c r="E45">
+      <c r="F46">
         <v>0.77280000000000015</v>
       </c>
-      <c r="F45">
+      <c r="G46">
         <v>0.30296000000000001</v>
       </c>
-      <c r="G45">
+      <c r="H46">
         <v>1.0794559999999997</v>
       </c>
-      <c r="H45">
+      <c r="I46">
         <v>0.30979200000000001</v>
       </c>
-      <c r="I45">
+      <c r="J46">
         <v>0.66315199999999996</v>
       </c>
-      <c r="J45">
+      <c r="K46">
         <v>0.440944</v>
       </c>
-      <c r="K45">
+      <c r="L46">
         <v>0.43825599999999992</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47">
         <v>79.044074999999992</v>
       </c>
-      <c r="B46">
+      <c r="C47">
         <v>4.9490099999999995</v>
       </c>
-      <c r="C46">
+      <c r="D47">
         <v>0.91574999999999995</v>
       </c>
-      <c r="D46">
+      <c r="E47">
         <v>2.0577149999999995</v>
       </c>
-      <c r="E46">
+      <c r="F47">
         <v>0.76823999999999992</v>
       </c>
-      <c r="F46">
+      <c r="G47">
         <v>0.21779999999999997</v>
       </c>
-      <c r="G46">
+      <c r="H47">
         <v>0.256245</v>
       </c>
-      <c r="H46">
+      <c r="I47">
         <v>0.34567499999999995</v>
       </c>
-      <c r="I46">
+      <c r="J47">
         <v>0.75619500000000006</v>
       </c>
-      <c r="J46">
+      <c r="K47">
         <v>1.05138</v>
       </c>
-      <c r="K46">
+      <c r="L47">
         <v>0.51463499999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48">
         <v>272.76352000000003</v>
       </c>
-      <c r="B47">
+      <c r="C48">
         <v>33.724800000000002</v>
       </c>
-      <c r="C47">
+      <c r="D48">
         <v>6.2077599999999995</v>
       </c>
-      <c r="D47">
+      <c r="E48">
         <v>12.952479999999998</v>
       </c>
-      <c r="E47">
+      <c r="F48">
         <v>5.1880799999999994</v>
       </c>
-      <c r="F47">
+      <c r="G48">
         <v>0.66135999999999984</v>
       </c>
-      <c r="G47">
+      <c r="H48">
         <v>4.5015999999999998</v>
       </c>
-      <c r="H47">
+      <c r="I48">
         <v>1.7117599999999995</v>
       </c>
-      <c r="I47">
+      <c r="J48">
         <v>1.53112</v>
       </c>
-      <c r="J47">
+      <c r="K48">
         <v>0.68144000000000005</v>
       </c>
-      <c r="K47">
+      <c r="L48">
         <v>1.20008</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49">
         <v>150.7345</v>
       </c>
-      <c r="B48">
+      <c r="C49">
         <v>12.113849999999999</v>
       </c>
-      <c r="C48">
+      <c r="D49">
         <v>2.2981000000000003</v>
       </c>
-      <c r="D48">
+      <c r="E49">
         <v>3.5780500000000002</v>
       </c>
-      <c r="E48">
+      <c r="F49">
         <v>1.4190750000000001</v>
       </c>
-      <c r="F48">
+      <c r="G49">
         <v>0.30887499999999996</v>
       </c>
-      <c r="G48">
+      <c r="H49">
         <v>1.4195999999999998</v>
       </c>
-      <c r="H48">
+      <c r="I49">
         <v>0.60707499999999992</v>
       </c>
-      <c r="I48">
+      <c r="J49">
         <v>0.91087499999999999</v>
       </c>
-      <c r="J48">
+      <c r="K49">
         <v>1.444275</v>
       </c>
-      <c r="K48">
+      <c r="L49">
         <v>2.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50">
         <v>419.47581000000002</v>
       </c>
-      <c r="B49">
+      <c r="C50">
         <v>48.494680000000002</v>
       </c>
-      <c r="C49">
+      <c r="D50">
         <v>10.54027</v>
       </c>
-      <c r="D49">
+      <c r="E50">
         <v>25.948000000000004</v>
       </c>
-      <c r="E49">
+      <c r="F50">
         <v>8.4726200000000009</v>
       </c>
-      <c r="F49">
+      <c r="G50">
         <v>1.82</v>
       </c>
-      <c r="G49">
+      <c r="H50">
         <v>6.2661299999999995</v>
       </c>
-      <c r="H49">
+      <c r="I50">
         <v>0.70277999999999996</v>
       </c>
-      <c r="I49">
+      <c r="J50">
         <v>3.3578999999999994</v>
       </c>
-      <c r="J49">
+      <c r="K50">
         <v>3.1298799999999996</v>
       </c>
-      <c r="K49">
+      <c r="L50">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51">
         <v>334.71970999999996</v>
       </c>
-      <c r="B50">
+      <c r="C51">
         <v>35.711910000000003</v>
       </c>
-      <c r="C50">
+      <c r="D51">
         <v>5.7043999999999997</v>
       </c>
-      <c r="D50">
+      <c r="E51">
         <v>15.379909999999999</v>
       </c>
-      <c r="E50">
+      <c r="F51">
         <v>4.8115599999999992</v>
       </c>
-      <c r="F50">
+      <c r="G51">
         <v>0.71409</v>
       </c>
-      <c r="G50">
+      <c r="H51">
         <v>3.2233500000000004</v>
       </c>
-      <c r="H50">
+      <c r="I51">
         <v>5.7834399999999997</v>
       </c>
-      <c r="I50">
+      <c r="J51">
         <v>0.11725999999999998</v>
       </c>
-      <c r="J50">
+      <c r="K51">
         <v>8.9390599999999996</v>
       </c>
-      <c r="K50">
+      <c r="L51">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52">
         <v>340.22169999999994</v>
       </c>
-      <c r="B51">
+      <c r="C52">
         <v>43.584969999999998</v>
       </c>
-      <c r="C51">
+      <c r="D52">
         <v>5.2072800000000008</v>
       </c>
-      <c r="D51">
+      <c r="E52">
         <v>17.608629999999998</v>
       </c>
-      <c r="E51">
+      <c r="F52">
         <v>5.1785499999999995</v>
       </c>
-      <c r="F51">
+      <c r="G52">
         <v>0.55080999999999991</v>
       </c>
-      <c r="G51">
+      <c r="H52">
         <v>2.4004500000000002</v>
       </c>
-      <c r="H51">
+      <c r="I52">
         <v>1.7159999999999997</v>
       </c>
-      <c r="I51">
+      <c r="J52">
         <v>0.45057999999999998</v>
-      </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>522.51940000000002</v>
-      </c>
-      <c r="B52">
-        <v>74.915749999999989</v>
-      </c>
-      <c r="C52">
-        <v>8.277099999999999</v>
-      </c>
-      <c r="D52">
-        <v>33.226309999999998</v>
-      </c>
-      <c r="E52">
-        <v>10.423919999999999</v>
-      </c>
-      <c r="F52">
-        <v>1.4697799999999999</v>
-      </c>
-      <c r="G52">
-        <v>6.1336599999999999</v>
-      </c>
-      <c r="H52">
-        <v>4.4803199999999999</v>
-      </c>
-      <c r="I52">
-        <v>0.63375000000000004</v>
-      </c>
-      <c r="J52">
-        <v>5.0709099999999987</v>
       </c>
       <c r="K52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53">
+        <v>522.51940000000002</v>
+      </c>
+      <c r="C53">
+        <v>74.915749999999989</v>
+      </c>
+      <c r="D53">
+        <v>8.277099999999999</v>
+      </c>
+      <c r="E53">
+        <v>33.226309999999998</v>
+      </c>
+      <c r="F53">
+        <v>10.423919999999999</v>
+      </c>
+      <c r="G53">
+        <v>1.4697799999999999</v>
+      </c>
+      <c r="H53">
+        <v>6.1336599999999999</v>
+      </c>
+      <c r="I53">
+        <v>4.4803199999999999</v>
+      </c>
+      <c r="J53">
+        <v>0.63375000000000004</v>
+      </c>
+      <c r="K53">
+        <v>5.0709099999999987</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54">
         <v>535.61325999999997</v>
       </c>
-      <c r="B53">
+      <c r="C54">
         <v>79.909440000000004</v>
       </c>
-      <c r="C53">
+      <c r="D54">
         <v>8.0319199999999977</v>
       </c>
-      <c r="D53">
+      <c r="E54">
         <v>41.127449999999989</v>
       </c>
-      <c r="E53">
+      <c r="F54">
         <v>12.630929999999999</v>
       </c>
-      <c r="F53">
+      <c r="G54">
         <v>1.9190599999999998</v>
       </c>
-      <c r="G53">
+      <c r="H54">
         <v>13.069809999999999</v>
       </c>
-      <c r="H53">
+      <c r="I54">
         <v>1.5044899999999999</v>
       </c>
-      <c r="I53">
+      <c r="J54">
         <v>3.5306699999999998</v>
       </c>
-      <c r="J53">
+      <c r="K54">
         <v>9.0305800000000023</v>
       </c>
-      <c r="K53">
+      <c r="L54">
         <v>2.2313199999999993</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55">
         <v>369.66604999999998</v>
       </c>
-      <c r="B54">
+      <c r="C55">
         <v>51.827750000000002</v>
       </c>
-      <c r="C54">
+      <c r="D55">
         <v>5.48977</v>
       </c>
-      <c r="D54">
+      <c r="E55">
         <v>25.099230000000002</v>
       </c>
-      <c r="E54">
+      <c r="F55">
         <v>6.231679999999999</v>
       </c>
-      <c r="F54">
+      <c r="G55">
         <v>0.72214999999999996</v>
       </c>
-      <c r="G54">
+      <c r="H55">
         <v>5.2397799999999997</v>
       </c>
-      <c r="H54">
+      <c r="I55">
         <v>2.7104999999999997</v>
       </c>
-      <c r="I54">
+      <c r="J55">
         <v>0.624</v>
       </c>
-      <c r="J54">
+      <c r="K55">
         <v>6.9824299999999999</v>
       </c>
-      <c r="K54">
+      <c r="L55">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56">
         <v>294.06662999999998</v>
       </c>
-      <c r="B55">
+      <c r="C56">
         <v>41.019029999999994</v>
       </c>
-      <c r="C55">
+      <c r="D56">
         <v>5.0492000000000008</v>
       </c>
-      <c r="D55">
+      <c r="E56">
         <v>20.33681</v>
       </c>
-      <c r="E55">
+      <c r="F56">
         <v>6.174739999999999</v>
       </c>
-      <c r="F55">
+      <c r="G56">
         <v>0.82731999999999994</v>
       </c>
-      <c r="G55">
+      <c r="H56">
         <v>5.5662099999999999</v>
       </c>
-      <c r="H55">
+      <c r="I56">
         <v>2.5390300000000003</v>
       </c>
-      <c r="I55">
+      <c r="J56">
         <v>0.45877000000000001</v>
       </c>
-      <c r="J55">
+      <c r="K56">
         <v>2.1200400000000004</v>
       </c>
-      <c r="K55">
+      <c r="L56">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57">
         <v>252.83153999999999</v>
       </c>
-      <c r="B56">
+      <c r="C57">
         <v>35.398089999999996</v>
       </c>
-      <c r="C56">
+      <c r="D57">
         <v>4.3924399999999997</v>
       </c>
-      <c r="D56">
+      <c r="E57">
         <v>17.995900000000002</v>
       </c>
-      <c r="E56">
+      <c r="F57">
         <v>5.2753999999999994</v>
       </c>
-      <c r="F56">
+      <c r="G57">
         <v>0.40546999999999994</v>
       </c>
-      <c r="G56">
+      <c r="H57">
         <v>5.115759999999999</v>
       </c>
-      <c r="H56">
+      <c r="I57">
         <v>1.3365299999999998</v>
       </c>
-      <c r="I56">
+      <c r="J57">
         <v>2.79006</v>
       </c>
-      <c r="J56">
+      <c r="K57">
         <v>7.4115599999999988</v>
       </c>
-      <c r="K56">
+      <c r="L57">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58">
         <v>247.14156999999997</v>
       </c>
-      <c r="B57">
+      <c r="C58">
         <v>30.79297</v>
       </c>
-      <c r="C57">
+      <c r="D58">
         <v>2.9642599999999999</v>
       </c>
-      <c r="D57">
+      <c r="E58">
         <v>15.190629999999999</v>
       </c>
-      <c r="E57">
+      <c r="F58">
         <v>3.3924800000000004</v>
       </c>
-      <c r="F57">
+      <c r="G58">
         <v>1.6756999999999995</v>
       </c>
-      <c r="G57">
+      <c r="H58">
         <v>11.207820000000002</v>
       </c>
-      <c r="H57">
+      <c r="I58">
         <v>2.5817999999999999</v>
       </c>
-      <c r="I57">
+      <c r="J58">
         <v>3.9846299999999997</v>
       </c>
-      <c r="J57">
+      <c r="K58">
         <v>13.912469999999999</v>
       </c>
-      <c r="K57">
+      <c r="L58">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59">
         <v>409.03823999999992</v>
       </c>
-      <c r="B58">
+      <c r="C59">
         <v>68.587609999999984</v>
       </c>
-      <c r="C58">
+      <c r="D59">
         <v>8.5386599999999984</v>
       </c>
-      <c r="D58">
+      <c r="E59">
         <v>35.384700000000002</v>
       </c>
-      <c r="E58">
+      <c r="F59">
         <v>12.559429999999999</v>
       </c>
-      <c r="F58">
+      <c r="G59">
         <v>3.0616300000000001</v>
       </c>
-      <c r="G58">
+      <c r="H59">
         <v>12.534339999999998</v>
       </c>
-      <c r="H58">
+      <c r="I59">
         <v>1.4747199999999998</v>
       </c>
-      <c r="I58">
+      <c r="J59">
         <v>2.40448</v>
       </c>
-      <c r="J58">
+      <c r="K59">
         <v>4.2091400000000005</v>
       </c>
-      <c r="K58">
+      <c r="L59">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60">
         <v>484.99398999999994</v>
       </c>
-      <c r="B59">
+      <c r="C60">
         <v>58.001579999999997</v>
       </c>
-      <c r="C59">
+      <c r="D60">
         <v>5.8713199999999999</v>
       </c>
-      <c r="D59">
+      <c r="E60">
         <v>30.743569999999998</v>
       </c>
-      <c r="E59">
+      <c r="F60">
         <v>6.79237</v>
       </c>
-      <c r="F59">
+      <c r="G60">
         <v>1.4344199999999998</v>
       </c>
-      <c r="G59">
+      <c r="H60">
         <v>9.4174599999999984</v>
       </c>
-      <c r="H59">
+      <c r="I60">
         <v>1.7994599999999998</v>
       </c>
-      <c r="I59">
+      <c r="J60">
         <v>4.7547499999999996</v>
       </c>
-      <c r="J59">
+      <c r="K60">
         <v>5.8081399999999999</v>
       </c>
-      <c r="K59">
+      <c r="L60">
         <v>2.3555999999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61">
         <v>307.74587999999994</v>
       </c>
-      <c r="B60">
+      <c r="C61">
         <v>50.193000000000005</v>
       </c>
-      <c r="C60">
+      <c r="D61">
         <v>5.2726699999999997</v>
       </c>
-      <c r="D60">
+      <c r="E61">
         <v>31.122389999999999</v>
       </c>
-      <c r="E60">
+      <c r="F61">
         <v>11.571820000000001</v>
       </c>
-      <c r="F60">
+      <c r="G61">
         <v>3.3792200000000001</v>
       </c>
-      <c r="G60">
+      <c r="H61">
         <v>12.521339999999999</v>
       </c>
-      <c r="H60">
+      <c r="I61">
         <v>4.7888099999999998</v>
       </c>
-      <c r="I60">
+      <c r="J61">
         <v>3.7774100000000002</v>
       </c>
-      <c r="J60">
+      <c r="K61">
         <v>4.4652400000000005</v>
       </c>
-      <c r="K60">
+      <c r="L61">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62">
         <v>216.15710999999996</v>
       </c>
-      <c r="B61">
+      <c r="C62">
         <v>37.672309999999996</v>
       </c>
-      <c r="C61">
+      <c r="D62">
         <v>4.7564400000000004</v>
       </c>
-      <c r="D61">
+      <c r="E62">
         <v>28.691520000000004</v>
       </c>
-      <c r="E61">
+      <c r="F62">
         <v>7.0783699999999996</v>
       </c>
-      <c r="F61">
+      <c r="G62">
         <v>2.2513400000000003</v>
       </c>
-      <c r="G61">
+      <c r="H62">
         <v>14.994199999999996</v>
       </c>
-      <c r="H61">
+      <c r="I62">
         <v>0.96265000000000001</v>
       </c>
-      <c r="I61">
+      <c r="J62">
         <v>1.48187</v>
       </c>
-      <c r="J61">
+      <c r="K62">
         <v>3.6953799999999997</v>
       </c>
-      <c r="K61">
+      <c r="L62">
         <v>7.8075400000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63">
         <v>1929.29269</v>
       </c>
-      <c r="B62">
+      <c r="C63">
         <v>372.67073999999997</v>
       </c>
-      <c r="C62">
+      <c r="D63">
         <v>42.614519999999999</v>
       </c>
-      <c r="D62">
+      <c r="E63">
         <v>208.40481999999997</v>
       </c>
-      <c r="E62">
+      <c r="F63">
         <v>64.680980000000005</v>
       </c>
-      <c r="F62">
+      <c r="G63">
         <v>16.90091</v>
       </c>
-      <c r="G62">
+      <c r="H63">
         <v>87.113649999999993</v>
       </c>
-      <c r="H62">
+      <c r="I63">
         <v>22.91835</v>
       </c>
-      <c r="I62">
+      <c r="J63">
         <v>11.382150000000001</v>
       </c>
-      <c r="J62">
+      <c r="K63">
         <v>22.101299999999998</v>
       </c>
-      <c r="K62">
+      <c r="L63">
         <v>25.780169999999995</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64">
         <v>455.79169999999988</v>
       </c>
-      <c r="B63">
+      <c r="C64">
         <v>113.61102999999997</v>
       </c>
-      <c r="C63">
+      <c r="D64">
         <v>10.633609999999999</v>
       </c>
-      <c r="D63">
+      <c r="E64">
         <v>93.909009999999995</v>
       </c>
-      <c r="E63">
+      <c r="F64">
         <v>17.412849999999999</v>
       </c>
-      <c r="F63">
+      <c r="G64">
         <v>7.9141399999999988</v>
       </c>
-      <c r="G63">
+      <c r="H64">
         <v>50.785670000000003</v>
       </c>
-      <c r="H63">
+      <c r="I64">
         <v>4.4733000000000001</v>
       </c>
-      <c r="I63">
+      <c r="J64">
         <v>3.5885200000000004</v>
       </c>
-      <c r="J63">
+      <c r="K64">
         <v>27.629420000000003</v>
       </c>
-      <c r="K63">
+      <c r="L64">
         <v>4.5663799999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65">
         <v>435.10792000000004</v>
       </c>
-      <c r="B64">
+      <c r="C65">
         <v>18.155799999999999</v>
       </c>
-      <c r="C64">
+      <c r="D65">
         <v>7.3295299999999983</v>
       </c>
-      <c r="D64">
+      <c r="E65">
         <v>10.513489999999999</v>
       </c>
-      <c r="E64">
+      <c r="F65">
         <v>6.4661999999999997</v>
       </c>
-      <c r="F64">
+      <c r="G65">
         <v>1.2625599999999999</v>
       </c>
-      <c r="G64">
+      <c r="H65">
         <v>3.88869</v>
       </c>
-      <c r="H64">
+      <c r="I65">
         <v>8.0788499999999974</v>
       </c>
-      <c r="I64">
+      <c r="J65">
         <v>19.234279999999998</v>
       </c>
-      <c r="J64">
+      <c r="K65">
         <v>0</v>
       </c>
-      <c r="K64">
+      <c r="L65">
         <v>0</v>
       </c>
     </row>

</xml_diff>